<commit_message>
Adjective & Noun models added
</commit_message>
<xml_diff>
--- a/api_test_files/mixed.xlsx
+++ b/api_test_files/mixed.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k1l77\Desktop\Diploma\api_test_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k1l77\DisGen\api_test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8BB06F4-8587-4BAD-A451-04CAA4009E1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D45F6A-7694-41C9-82B4-98BC71339102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5620329B-1BD3-4BC6-94DE-FB319552D40C}"/>
   </bookViews>
@@ -12706,7 +12706,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" customWidth="1"/>
     <col min="2" max="2" width="74.85546875" customWidth="1"/>
     <col min="3" max="3" width="38.28515625" customWidth="1"/>
     <col min="4" max="4" width="23.140625" customWidth="1"/>

</xml_diff>